<commit_message>
edit load clean ASA24
</commit_message>
<xml_diff>
--- a/eg_data/VVKAJ/ind_metadata_prep.xlsx
+++ b/eg_data/VVKAJ/ind_metadata_prep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\dietary_patterns\eg_data\VVKAJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\VVKAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAC5A5-2126-406A-A111-433A9DE9D84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57EF81E-2B2A-4F1F-9E9D-EC82D65DCD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20880" yWindow="-2985" windowWidth="20145" windowHeight="12315" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21630" yWindow="-2490" windowWidth="24225" windowHeight="12705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="90">
   <si>
     <t>UserName</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>SampleID</t>
+  </si>
+  <si>
+    <t>VVKAJ117</t>
+  </si>
+  <si>
+    <t>vvkaj.00049</t>
+  </si>
+  <si>
+    <t>vvkaj.00050</t>
+  </si>
+  <si>
+    <t>vvkaj.00051</t>
   </si>
 </sst>
 </file>
@@ -1923,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E71D65E-2D67-4DC7-8DD0-207ABB2ACAEE}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,6 +2388,32 @@
         <v>91</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>76</v>
+      </c>
+      <c r="F18">
+        <v>175</v>
+      </c>
+      <c r="G18">
+        <v>24.816326530612244</v>
+      </c>
+      <c r="H18">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
     <sortCondition ref="A2:A17"/>
@@ -2383,16 +2421,17 @@
     <sortCondition ref="C2:C17"/>
     <sortCondition ref="F2:F17"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594EDA6F-1CFC-42B1-90D7-9924266EEBF7}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3973,6 +4012,102 @@
         <v>91</v>
       </c>
     </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="19">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>23</v>
+      </c>
+      <c r="G50">
+        <v>76</v>
+      </c>
+      <c r="H50">
+        <v>175</v>
+      </c>
+      <c r="I50">
+        <v>24.816326530612244</v>
+      </c>
+      <c r="J50">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="20">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>23</v>
+      </c>
+      <c r="G51">
+        <v>76</v>
+      </c>
+      <c r="H51">
+        <v>175</v>
+      </c>
+      <c r="I51">
+        <v>24.816326530612244</v>
+      </c>
+      <c r="J51">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="20">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>23</v>
+      </c>
+      <c r="G52">
+        <v>76</v>
+      </c>
+      <c r="H52">
+        <v>175</v>
+      </c>
+      <c r="I52">
+        <v>24.816326530612244</v>
+      </c>
+      <c r="J52">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J49">
     <sortCondition ref="B2:B49"/>
@@ -3984,10 +4119,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEA0401-A6D3-450D-B73D-29B36405E30A}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,17 +4221,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBECE233-8A82-485F-BD4D-7571C7A76DC4}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4520,7 +4661,34 @@
         <v>91</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17">
+        <v>76</v>
+      </c>
+      <c r="F17">
+        <v>175</v>
+      </c>
+      <c r="G17">
+        <v>24.816326530612244</v>
+      </c>
+      <c r="H17">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>